<commit_message>
Remove SSID from Mass Upload
</commit_message>
<xml_diff>
--- a/public/docs/roboplay_scoreboard_student_upload_template.xlsx
+++ b/public/docs/roboplay_scoreboard_student_upload_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lamp\scoreboard\public\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lamp\scoreboard2\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{39F72BE3-E5A1-49D7-8BE8-41A01C52399F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="21075" windowHeight="10545"/>
+    <workbookView xWindow="1620" yWindow="855" windowWidth="17115" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>First Name</t>
   </si>
@@ -33,9 +34,6 @@
   </si>
   <si>
     <t>Last Name</t>
-  </si>
-  <si>
-    <t>SSID</t>
   </si>
   <si>
     <t>Ethnicity</t>
@@ -155,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,7 +246,176 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="13">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -265,193 +432,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -477,9 +457,9 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="13"/>
-      <tableStyleElement type="headerRow" dxfId="12"/>
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -510,7 +490,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -619,7 +605,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Fill out all  9 columns for each student.  Student E-mail and T-Shirt Size fields are optional and may be left blank.</a:t>
+            <a:t>Fill out all  8 columns for each student.  Student E-mail and T-Shirt Size fields are optional and may be left blank.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -901,7 +887,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -958,19 +950,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J30" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="11">
-  <autoFilter ref="A1:J30"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="First Name" dataDxfId="10"/>
-    <tableColumn id="2" name="Middle/Nick Name" dataDxfId="9"/>
-    <tableColumn id="3" name="Last Name" dataDxfId="8"/>
-    <tableColumn id="4" name="Gender" dataDxfId="7"/>
-    <tableColumn id="5" name="SSID" dataDxfId="6"/>
-    <tableColumn id="6" name="Ethnicity" dataDxfId="5"/>
-    <tableColumn id="7" name="Grade" dataDxfId="4"/>
-    <tableColumn id="8" name="Math Level" dataDxfId="3"/>
-    <tableColumn id="9" name="T-Shirt" dataDxfId="2"/>
-    <tableColumn id="10" name="E-mail" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I30" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:I30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="First Name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Middle/Nick Name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Last Name" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Gender" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ethnicity" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Grade" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Math Level" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="T-Shirt" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="E-mail" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1052,6 +1043,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1087,6 +1095,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1262,7 +1287,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1280,26 +1305,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1336,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1319,83 +1345,74 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1234567891</v>
-      </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="F3" s="1">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3216549877</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1">
-        <v>6</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1404,10 +1421,9 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1417,9 +1433,8 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1429,9 +1444,8 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1441,9 +1455,8 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1453,9 +1466,8 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1465,9 +1477,8 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1477,9 +1488,8 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1489,9 +1499,8 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1501,9 +1510,8 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1513,9 +1521,8 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1525,9 +1532,8 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1537,9 +1543,8 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1549,9 +1554,8 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1561,9 +1565,8 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1573,9 +1576,8 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1585,9 +1587,8 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1597,9 +1598,8 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1609,9 +1609,8 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1621,9 +1620,8 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1633,9 +1631,8 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1645,9 +1642,8 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1657,9 +1653,8 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1669,9 +1664,8 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1681,9 +1675,8 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1693,9 +1686,8 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1705,9 +1697,8 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1717,31 +1708,26 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warming" error="You must select from the list of Ethnicities" sqref="F2:F30">
+  <dataValidations count="4">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warming" error="You must select from the list of Ethnicities" sqref="E2:E30" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"American Indian or Alaskan Native,Asian,Hispanic or Latino,Black or African-American,Native Hawaiian or Other Pacific Islander,White,Other"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Student ID" error="Student ID must be 10 digits and numeric." sqref="E2:E30">
-      <formula1>999999999</formula1>
-      <formula2>10000000000</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Grade" error="Grade must be between 5th and 14th." promptTitle="Enter Grade" prompt="Grade must be between 4th and 14th." sqref="G2:G30">
+    <dataValidation type="decimal" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Grade" error="Grade must be between 5th and 14th." promptTitle="Enter Grade" prompt="Grade must be between 4th and 14th." sqref="F2:F30" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>5</formula1>
       <formula2>14</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid T-Shirt Size" error="Size must be one of XS,S,M,L, or XL." promptTitle="Enter T-Shirt Size" prompt="Size must be one of XS,S,M,L, or XL" sqref="I2:I30">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid T-Shirt Size" error="Size must be one of XS,S,M,L, or XL." promptTitle="Enter T-Shirt Size" prompt="Size must be one of XS,S,M,L, or XL" sqref="H2:H30" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"XS,S,M,L,XL"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1751,11 +1737,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Grade" error="Please choose from the list." promptTitle="Math Level" prompt="Select the studen Math Level">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Grade" error="Please choose from the list." promptTitle="Math Level" prompt="Select the studen Math Level" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>'Math Levels'!$A$1:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H30</xm:sqref>
+          <xm:sqref>G2:G30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1764,7 +1750,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A18"/>
   <sheetViews>
@@ -1779,92 +1765,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>